<commit_message>
added lp20 connectors to karca bom
</commit_message>
<xml_diff>
--- a/doc/kARCA - Complete BOM.xlsx
+++ b/doc/kARCA - Complete BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amyda\dev\karca\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CBE83C-5380-454D-8CEC-2C41A2D013DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955CD716-CC74-4EE2-8380-6C6DBD9F288F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14136" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="121">
   <si>
     <t>GRAND TOTAL:</t>
   </si>
@@ -393,6 +393,15 @@
   </si>
   <si>
     <t>https://www.amazon.com/GDQLCNXB-Speaker-Microphone-Connector-Housing/dp/B0B1X4JXYX/ref=sr_1_8?crid=3GY0BVESAS9W4&amp;keywords=5+pin+female+xlr+connector&amp;qid=1673269882&amp;sprefix=pin+female+xlr+connector%2Caps%2C194&amp;sr=8-8</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/CNLINKO-waterproof-connector-locking-connect/dp/B07WJRWCJ2/ref=sr_1_5?content-id=amzn1.sym.dbb2bd15-326d-4d11-831d-f6e882ac5d1f&amp;keywords=cnlinko%2B2%2Bpin&amp;pd_rd_r=ed196329-f6c7-47e5-97d3-2de5f7de37a1&amp;pd_rd_w=St1vx&amp;pd_rd_wg=TvEb6&amp;pf_rd_p=dbb2bd15-326d-4d11-831d-f6e882ac5d1f&amp;pf_rd_r=FSPHWPQT51AVNV7YFP9Y&amp;qid=1673389576&amp;sr=8-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>2-pin LP20 connector set</t>
+  </si>
+  <si>
+    <t>CNLINKO</t>
   </si>
 </sst>
 </file>
@@ -981,8 +990,8 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <f>Box!I18+'PCB (assembled by Eclipse)'!I24</f>
-        <v>351.65000000000003</v>
+        <f>Box!I19+'PCB (assembled by Eclipse)'!I24</f>
+        <v>415.6099999999999</v>
       </c>
     </row>
   </sheetData>
@@ -993,11 +1002,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1143,43 +1152,59 @@
     </row>
     <row r="4" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="20">
+        <v>15.99</v>
+      </c>
+      <c r="F4" s="21">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
+        <v>3</v>
+      </c>
+      <c r="H4" s="21">
+        <v>4</v>
+      </c>
+      <c r="I4" s="20">
+        <v>63.96</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+    </row>
+    <row r="5" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="A5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E5" s="24">
         <v>5</v>
-      </c>
-      <c r="F4" s="23">
-        <v>1</v>
-      </c>
-      <c r="G4" s="23">
-        <v>1</v>
-      </c>
-      <c r="H4" s="23">
-        <v>1</v>
-      </c>
-      <c r="I4" s="24">
-        <f t="shared" ref="I2:I7" si="0">H4*E4</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="23" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="24">
-        <v>115.99</v>
       </c>
       <c r="F5" s="23">
         <v>1</v>
@@ -1191,45 +1216,44 @@
         <v>1</v>
       </c>
       <c r="I5" s="24">
+        <f t="shared" ref="I5:I8" si="0">H5*E5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="23" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="24">
+        <v>115.99</v>
+      </c>
+      <c r="F6" s="23">
+        <v>1</v>
+      </c>
+      <c r="G6" s="23">
+        <v>1</v>
+      </c>
+      <c r="H6" s="23">
+        <v>1</v>
+      </c>
+      <c r="I6" s="24">
         <f t="shared" si="0"/>
         <v>115.99</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K6" s="25" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="A6" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="24">
-        <v>14.46</v>
-      </c>
-      <c r="F6" s="23">
-        <v>100</v>
-      </c>
-      <c r="G6" s="23">
-        <v>4</v>
-      </c>
-      <c r="H6" s="23">
-        <f>CEILING(G6/F6,1)</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="24">
-        <f t="shared" si="0"/>
-        <v>14.46</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
@@ -1237,19 +1261,19 @@
         <v>23</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" s="24">
-        <v>6.18</v>
+        <v>14.46</v>
       </c>
       <c r="F7" s="23">
         <v>100</v>
       </c>
       <c r="G7" s="23">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="H7" s="23">
         <f>CEILING(G7/F7,1)</f>
@@ -1257,64 +1281,65 @@
       </c>
       <c r="I7" s="24">
         <f t="shared" si="0"/>
+        <v>14.46</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="A8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="24">
         <v>6.18</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="F8" s="23">
+        <v>100</v>
+      </c>
+      <c r="G8" s="23">
+        <v>36</v>
+      </c>
+      <c r="H8" s="23">
+        <f>CEILING(G8/F8,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="24">
+        <f t="shared" si="0"/>
+        <v>6.18</v>
+      </c>
+      <c r="J8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="23" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="A8" s="27" t="s">
+    <row r="9" spans="1:26" s="23" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="A9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="24">
-        <v>18.75</v>
-      </c>
-      <c r="F9" s="23">
-        <v>1</v>
-      </c>
-      <c r="G9" s="23">
-        <v>1</v>
-      </c>
-      <c r="H9" s="23">
-        <v>1</v>
-      </c>
-      <c r="I9" s="24">
-        <f>25*0.75</f>
-        <v>18.75</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>34</v>
-      </c>
+      <c r="E9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="24">
-        <v>3.58</v>
+        <v>18.75</v>
       </c>
       <c r="F10" s="23">
         <v>1</v>
@@ -1326,11 +1351,11 @@
         <v>1</v>
       </c>
       <c r="I10" s="24">
-        <f>H10*E10</f>
-        <v>3.58</v>
+        <f>25*0.75</f>
+        <v>18.75</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
@@ -1341,7 +1366,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="24">
         <v>3.58</v>
@@ -1371,7 +1396,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="24">
         <v>3.58</v>
@@ -1401,7 +1426,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="24">
         <v>3.58</v>
@@ -1431,7 +1456,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="24">
         <v>3.58</v>
@@ -1454,114 +1479,140 @@
       </c>
     </row>
     <row r="15" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="E15" s="24"/>
-      <c r="I15" s="24"/>
+      <c r="A15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="24">
+        <v>3.58</v>
+      </c>
+      <c r="F15" s="23">
+        <v>1</v>
+      </c>
+      <c r="G15" s="23">
+        <v>1</v>
+      </c>
+      <c r="H15" s="23">
+        <v>1</v>
+      </c>
+      <c r="I15" s="24">
+        <f>H15*E15</f>
+        <v>3.58</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="A16" s="19" t="s">
+      <c r="E16" s="24"/>
+      <c r="I16" s="24"/>
+    </row>
+    <row r="17" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="A17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E17" s="20">
         <v>15.98</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="28">
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="28">
         <v>15.98</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="22" t="s">
+      <c r="J17" s="19"/>
+      <c r="K17" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="19"/>
-      <c r="W16" s="19"/>
-      <c r="X16" s="19"/>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="19"/>
-    </row>
-    <row r="17" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="E17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="5:9" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+    </row>
+    <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E18" s="2"/>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:26" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="E19" s="2"/>
+      <c r="H19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="3">
-        <f>SUM(I2:I17)</f>
-        <v>232.42000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="E19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="I19" s="3">
+        <f>SUM(I2:I18)</f>
+        <v>296.37999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E32" s="2"/>
       <c r="I32" s="2"/>
     </row>
@@ -5441,18 +5492,22 @@
       <c r="E1001" s="2"/>
       <c r="I1001" s="2"/>
     </row>
+    <row r="1002" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="E1002" s="2"/>
+      <c r="I1002" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="K6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="K7" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="K9" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="K10" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="K11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="K12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="K13" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="K14" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="K16" r:id="rId10" xr:uid="{7BD40A4C-5026-466A-A5E3-0545510372A6}"/>
+    <hyperlink ref="K6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="K10" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="K11" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="K12" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="K13" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="K14" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="K15" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="K17" r:id="rId10" xr:uid="{7BD40A4C-5026-466A-A5E3-0545510372A6}"/>
     <hyperlink ref="K2" r:id="rId11" xr:uid="{0AF5AA1C-10A5-4355-B3C0-B18C992E59DD}"/>
     <hyperlink ref="K3" r:id="rId12" xr:uid="{6CFD281E-DD41-4923-99C6-78F98A6E0E79}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
added jd1912 type relay for ignition to karca bom
</commit_message>
<xml_diff>
--- a/doc/kARCA - Complete BOM.xlsx
+++ b/doc/kARCA - Complete BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amyda\dev\karca\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955CD716-CC74-4EE2-8380-6C6DBD9F288F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B4490E-D011-409A-9672-4C82004DEB84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14136" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="125">
   <si>
     <t>GRAND TOTAL:</t>
   </si>
@@ -403,6 +403,18 @@
   <si>
     <t>CNLINKO</t>
   </si>
+  <si>
+    <t>https://www.amazon.com/ARTGEAR-Harness-Color-Labeled-Automotive-Motorcycle/dp/B078T8CMF6?th=1</t>
+  </si>
+  <si>
+    <t>The other one will be used on Labjack</t>
+  </si>
+  <si>
+    <t>Gebildet</t>
+  </si>
+  <si>
+    <t>JD1912 Car Relay Harness 12V 40A</t>
+  </si>
 </sst>
 </file>
 
@@ -540,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -594,6 +606,7 @@
     <xf numFmtId="6" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -990,8 +1003,8 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <f>Box!I19+'PCB (assembled by Eclipse)'!I24</f>
-        <v>415.6099999999999</v>
+        <f>Box!I20+'PCB (assembled by Eclipse)'!I24</f>
+        <v>424.09999999999991</v>
       </c>
     </row>
   </sheetData>
@@ -1002,11 +1015,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1321,55 +1334,57 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="23" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="A9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="24">
+        <v>8.49</v>
+      </c>
+      <c r="F9" s="23">
+        <v>2</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1</v>
+      </c>
+      <c r="H9" s="23">
+        <v>1</v>
+      </c>
+      <c r="I9" s="24">
+        <v>8.49</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="23" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A10" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="A10" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="24">
-        <v>18.75</v>
-      </c>
-      <c r="F10" s="23">
-        <v>1</v>
-      </c>
-      <c r="G10" s="23">
-        <v>1</v>
-      </c>
-      <c r="H10" s="23">
-        <v>1</v>
-      </c>
-      <c r="I10" s="24">
-        <f>25*0.75</f>
-        <v>18.75</v>
-      </c>
-      <c r="K10" s="26" t="s">
-        <v>34</v>
-      </c>
+      <c r="E10" s="24"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="24">
-        <v>3.58</v>
+        <v>18.75</v>
       </c>
       <c r="F11" s="23">
         <v>1</v>
@@ -1381,11 +1396,11 @@
         <v>1</v>
       </c>
       <c r="I11" s="24">
-        <f>H11*E11</f>
-        <v>3.58</v>
+        <f>25*0.75</f>
+        <v>18.75</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
@@ -1396,7 +1411,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="24">
         <v>3.58</v>
@@ -1426,7 +1441,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="24">
         <v>3.58</v>
@@ -1456,7 +1471,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="24">
         <v>3.58</v>
@@ -1486,7 +1501,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="24">
         <v>3.58</v>
@@ -1509,64 +1524,90 @@
       </c>
     </row>
     <row r="16" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="E16" s="24"/>
-      <c r="I16" s="24"/>
+      <c r="A16" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="24">
+        <v>3.58</v>
+      </c>
+      <c r="F16" s="23">
+        <v>1</v>
+      </c>
+      <c r="G16" s="23">
+        <v>1</v>
+      </c>
+      <c r="H16" s="23">
+        <v>1</v>
+      </c>
+      <c r="I16" s="24">
+        <f>H16*E16</f>
+        <v>3.58</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="A17" s="19" t="s">
+      <c r="E17" s="24"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="1:26" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="A18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E18" s="20">
         <v>15.98</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="28">
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="28">
         <v>15.98</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="22" t="s">
+      <c r="J18" s="19"/>
+      <c r="K18" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19"/>
-      <c r="X17" s="19"/>
-      <c r="Y17" s="19"/>
-      <c r="Z17" s="19"/>
-    </row>
-    <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="E18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:26" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+    </row>
+    <row r="19" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E19" s="2"/>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:26" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="E20" s="2"/>
+      <c r="H20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="3">
-        <f>SUM(I2:I18)</f>
-        <v>296.37999999999994</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
-      <c r="E20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="3">
+        <f>SUM(I2:I19)</f>
+        <v>304.86999999999995</v>
+      </c>
     </row>
     <row r="21" spans="1:26" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E21" s="2"/>
@@ -5495,24 +5536,29 @@
     <row r="1002" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
       <c r="E1002" s="2"/>
       <c r="I1002" s="2"/>
+    </row>
+    <row r="1003" spans="5:9" ht="13.8" x14ac:dyDescent="0.45">
+      <c r="E1003" s="2"/>
+      <c r="I1003" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="K7" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="K8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="K10" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="K11" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="K12" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="K13" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="K14" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="K15" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="K17" r:id="rId10" xr:uid="{7BD40A4C-5026-466A-A5E3-0545510372A6}"/>
+    <hyperlink ref="K11" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="K12" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="K13" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="K14" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="K15" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="K16" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="K18" r:id="rId10" xr:uid="{7BD40A4C-5026-466A-A5E3-0545510372A6}"/>
     <hyperlink ref="K2" r:id="rId11" xr:uid="{0AF5AA1C-10A5-4355-B3C0-B18C992E59DD}"/>
     <hyperlink ref="K3" r:id="rId12" xr:uid="{6CFD281E-DD41-4923-99C6-78F98A6E0E79}"/>
+    <hyperlink ref="K9" r:id="rId13" xr:uid="{37CBFB4F-E900-405E-B728-355733A21812}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>